<commit_message>
Changing art start date to EpisodeOfCare resource
</commit_message>
<xml_diff>
--- a/CodeSystem-SzClinicalObservationCodesCS.xlsx
+++ b/CodeSystem-SzClinicalObservationCodesCS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-10T08:40:27+00:00</t>
+    <t>2025-09-10T10:05:20+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -118,7 +118,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>13</t>
+    <t>11</t>
   </si>
   <si>
     <t>Level</t>
@@ -146,18 +146,6 @@
   </si>
   <si>
     <t>TPT Outcome</t>
-  </si>
-  <si>
-    <t>tpt-start-date</t>
-  </si>
-  <si>
-    <t>TPT Start Date</t>
-  </si>
-  <si>
-    <t>tpt-stop-date</t>
-  </si>
-  <si>
-    <t>TPT Stop Date</t>
   </si>
   <si>
     <t>art-regimen</t>
@@ -520,7 +508,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -672,30 +660,6 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13">
-      <c r="A13" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="B13" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="C13" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="B14" t="s" s="2">
-        <v>64</v>
-      </c>
-      <c r="C14" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="D14" s="2"/>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>